<commit_message>
git: fixed corrupted git commit; technical: crossing logic for landslide and liquefaction, landslide examples, updated datasets, improved preprocess, improved risk calculation, fixed some pipe strain models, cleaned up some scripts, zipped preprocessed IM for state network, untracked indiv. files, added command to extract in preprocessing
</commit_message>
<xml_diff>
--- a/param_dist/below_ground.xlsx
+++ b/param_dist/below_ground.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://slategeotech-my.sharepoint.com/personal/bzheng_slategeotech_com/Documents/CEC/OpenSRA/param_dist/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="187" documentId="13_ncr:1_{48A64A16-839D-4EB3-BF2F-A973C4A4B7ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A2E73DFD-1713-4CBF-A060-65AAE37B8B11}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{A3D454CB-C675-440C-B26E-BB3C7CD09156}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{36C11FD3-27ED-4E67-907E-D377D51E5187}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{0CF1B192-5A29-435B-821A-1A8E6C927DCF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{0CF1B192-5A29-435B-821A-1A8E6C927DCF}"/>
   </bookViews>
   <sheets>
     <sheet name="level1" sheetId="1" r:id="rId1"/>
@@ -128,7 +128,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="482" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="479" uniqueCount="91">
   <si>
     <t>normal</t>
   </si>
@@ -797,8 +797,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38878A27-4F03-488B-A8C6-4048A6415AE1}">
   <dimension ref="A1:K28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I28" sqref="I28"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I27" sqref="I27:J27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1647,10 +1647,10 @@
         <v>20</v>
       </c>
       <c r="I27">
-        <v>0</v>
+        <v>-180</v>
       </c>
       <c r="J27">
-        <v>180</v>
+        <v>360</v>
       </c>
       <c r="K27" t="s">
         <v>0</v>
@@ -1696,8 +1696,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF77FDDE-D87F-4E64-ADF5-F7C4C1229BC0}">
   <dimension ref="A1:K28"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1801,7 +1801,7 @@
         <v>70</v>
       </c>
       <c r="B4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C4" t="b">
         <v>1</v>
@@ -1812,8 +1812,8 @@
       <c r="E4" t="s">
         <v>5</v>
       </c>
-      <c r="F4" t="s">
-        <v>19</v>
+      <c r="F4">
+        <v>359000</v>
       </c>
       <c r="H4">
         <v>7.5</v>
@@ -1906,7 +1906,7 @@
         <v>100</v>
       </c>
       <c r="H7">
-        <v>70</v>
+        <v>90</v>
       </c>
       <c r="I7">
         <v>10</v>
@@ -2528,10 +2528,10 @@
         <v>20</v>
       </c>
       <c r="I27">
-        <v>0.1</v>
+        <v>-180</v>
       </c>
       <c r="J27">
-        <v>180</v>
+        <v>360</v>
       </c>
       <c r="K27" t="s">
         <v>0</v>
@@ -2577,7 +2577,7 @@
   <dimension ref="A1:K28"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="F7" sqref="F7:J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2679,7 +2679,7 @@
         <v>70</v>
       </c>
       <c r="B4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C4" t="b">
         <v>1</v>
@@ -2690,8 +2690,8 @@
       <c r="E4" t="s">
         <v>5</v>
       </c>
-      <c r="F4" t="s">
-        <v>19</v>
+      <c r="F4">
+        <v>359000</v>
       </c>
       <c r="H4">
         <v>7.5</v>
@@ -2780,11 +2780,11 @@
       <c r="E7" t="s">
         <v>3</v>
       </c>
-      <c r="F7" t="s">
-        <v>19</v>
+      <c r="F7">
+        <v>100</v>
       </c>
       <c r="H7">
-        <v>50</v>
+        <v>90</v>
       </c>
       <c r="I7">
         <v>10</v>
@@ -3048,7 +3048,7 @@
         <v>30</v>
       </c>
       <c r="B16" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C16" t="b">
         <v>0</v>
@@ -3060,7 +3060,7 @@
         <v>3</v>
       </c>
       <c r="F16" t="s">
-        <v>19</v>
+        <v>68</v>
       </c>
       <c r="H16">
         <v>20</v>
@@ -3199,7 +3199,7 @@
         <v>56</v>
       </c>
       <c r="B21" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C21" t="b">
         <v>0</v>
@@ -3211,7 +3211,7 @@
         <v>22</v>
       </c>
       <c r="F21" t="s">
-        <v>19</v>
+        <v>68</v>
       </c>
       <c r="H21">
         <v>5</v>
@@ -3353,7 +3353,7 @@
         <v>76</v>
       </c>
       <c r="B26" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C26" t="b">
         <v>0</v>
@@ -3365,7 +3365,7 @@
         <v>22</v>
       </c>
       <c r="F26" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="G26">
         <v>10</v>
@@ -3385,7 +3385,7 @@
         <v>77</v>
       </c>
       <c r="B27" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C27" t="b">
         <v>0</v>
@@ -3397,16 +3397,16 @@
         <v>22</v>
       </c>
       <c r="F27" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="G27">
         <v>20</v>
       </c>
       <c r="I27">
-        <v>0.1</v>
+        <v>-180</v>
       </c>
       <c r="J27">
-        <v>180</v>
+        <v>360</v>
       </c>
       <c r="K27" t="s">
         <v>0</v>
@@ -3417,7 +3417,7 @@
         <v>80</v>
       </c>
       <c r="B28" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C28" t="b">
         <v>0</v>
@@ -3429,7 +3429,7 @@
         <v>3</v>
       </c>
       <c r="F28" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="H28">
         <v>40</v>

</xml_diff>

<commit_message>
added examples for lateral spread, settlement, fault rupture; fixed algo for crossings; improved export format of results; updated methods param json for below ground
</commit_message>
<xml_diff>
--- a/param_dist/below_ground.xlsx
+++ b/param_dist/below_ground.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://slategeotech-my.sharepoint.com/personal/bzheng_slategeotech_com/Documents/CEC/OpenSRA/param_dist/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{A3D454CB-C675-440C-B26E-BB3C7CD09156}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{36C11FD3-27ED-4E67-907E-D377D51E5187}"/>
+  <xr:revisionPtr revIDLastSave="58" documentId="13_ncr:1_{A3D454CB-C675-440C-B26E-BB3C7CD09156}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D7F37046-9AD6-4F07-87ED-C9F62335E896}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{0CF1B192-5A29-435B-821A-1A8E6C927DCF}"/>
+    <workbookView xWindow="13905" yWindow="3975" windowWidth="23250" windowHeight="14055" activeTab="2" xr2:uid="{0CF1B192-5A29-435B-821A-1A8E6C927DCF}"/>
   </bookViews>
   <sheets>
     <sheet name="level1" sheetId="1" r:id="rId1"/>
@@ -128,7 +128,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="479" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="494" uniqueCount="92">
   <si>
     <t>normal</t>
   </si>
@@ -401,6 +401,9 @@
   </si>
   <si>
     <t>source for landslide deformation geometry: "none" for level 1, "CA landslide inventory" for level 2 and 3; users can also specify path to shapefile with geometries</t>
+  </si>
+  <si>
+    <t>theta_rake</t>
   </si>
 </sst>
 </file>
@@ -795,10 +798,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38878A27-4F03-488B-A8C6-4048A6415AE1}">
-  <dimension ref="A1:K28"/>
+  <dimension ref="A1:K29"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I27" sqref="I27:J27"/>
+      <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1295,7 +1298,7 @@
         <v>1</v>
       </c>
       <c r="C16" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D16" t="s">
         <v>36</v>
@@ -1683,6 +1686,38 @@
       </c>
       <c r="K28" t="s">
         <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>91</v>
+      </c>
+      <c r="B29" t="b">
+        <v>1</v>
+      </c>
+      <c r="C29" t="b">
+        <v>0</v>
+      </c>
+      <c r="D29" t="s">
+        <v>79</v>
+      </c>
+      <c r="E29" t="s">
+        <v>22</v>
+      </c>
+      <c r="F29" t="s">
+        <v>24</v>
+      </c>
+      <c r="G29">
+        <v>10</v>
+      </c>
+      <c r="I29">
+        <v>-360</v>
+      </c>
+      <c r="J29">
+        <v>360</v>
+      </c>
+      <c r="K29" t="s">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1694,10 +1729,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF77FDDE-D87F-4E64-ADF5-F7C4C1229BC0}">
-  <dimension ref="A1:K28"/>
+  <dimension ref="A1:K29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2176,7 +2211,7 @@
         <v>1</v>
       </c>
       <c r="C16" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D16" t="s">
         <v>36</v>
@@ -2564,6 +2599,38 @@
       </c>
       <c r="K28" t="s">
         <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>91</v>
+      </c>
+      <c r="B29" t="b">
+        <v>1</v>
+      </c>
+      <c r="C29" t="b">
+        <v>0</v>
+      </c>
+      <c r="D29" t="s">
+        <v>79</v>
+      </c>
+      <c r="E29" t="s">
+        <v>22</v>
+      </c>
+      <c r="F29" t="s">
+        <v>24</v>
+      </c>
+      <c r="G29">
+        <v>10</v>
+      </c>
+      <c r="I29">
+        <v>-360</v>
+      </c>
+      <c r="J29">
+        <v>360</v>
+      </c>
+      <c r="K29" t="s">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -2574,10 +2641,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68AD9398-98CA-4DC9-BCD5-D6EC9B94D5CB}">
-  <dimension ref="A1:K28"/>
+  <dimension ref="A1:K29"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7:J7"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="F16" activeCellId="1" sqref="F15 F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3051,7 +3118,7 @@
         <v>1</v>
       </c>
       <c r="C16" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D16" t="s">
         <v>36</v>
@@ -3060,7 +3127,7 @@
         <v>3</v>
       </c>
       <c r="F16" t="s">
-        <v>68</v>
+        <v>19</v>
       </c>
       <c r="H16">
         <v>20</v>
@@ -3439,6 +3506,38 @@
       </c>
       <c r="K28" t="s">
         <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>91</v>
+      </c>
+      <c r="B29" t="b">
+        <v>1</v>
+      </c>
+      <c r="C29" t="b">
+        <v>0</v>
+      </c>
+      <c r="D29" t="s">
+        <v>79</v>
+      </c>
+      <c r="E29" t="s">
+        <v>22</v>
+      </c>
+      <c r="F29" t="s">
+        <v>24</v>
+      </c>
+      <c r="G29">
+        <v>10</v>
+      </c>
+      <c r="I29">
+        <v>-360</v>
+      </c>
+      <c r="J29">
+        <v>360</v>
+      </c>
+      <c r="K29" t="s">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- fix error in pipe strain model - updated generic model examples
</commit_message>
<xml_diff>
--- a/param_dist/below_ground.xlsx
+++ b/param_dist/below_ground.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://slategeotech-my.sharepoint.com/personal/bzheng_slategeotech_com/Documents/CEC/OpenSRA/param_dist/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="61" documentId="13_ncr:1_{A3D454CB-C675-440C-B26E-BB3C7CD09156}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00E401F1-383E-4AE8-8CFF-2DB8FC46787D}"/>
+  <xr:revisionPtr revIDLastSave="74" documentId="13_ncr:1_{A3D454CB-C675-440C-B26E-BB3C7CD09156}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3AAC5B23-7A5E-4B88-99E3-AAC6E2F95A94}"/>
   <bookViews>
-    <workbookView xWindow="1290" yWindow="-120" windowWidth="27630" windowHeight="16440" activeTab="2" xr2:uid="{0CF1B192-5A29-435B-821A-1A8E6C927DCF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0CF1B192-5A29-435B-821A-1A8E6C927DCF}"/>
   </bookViews>
   <sheets>
     <sheet name="level1" sheetId="1" r:id="rId1"/>
@@ -799,8 +799,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38878A27-4F03-488B-A8C6-4048A6415AE1}">
   <dimension ref="A1:K29"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1248,7 +1248,7 @@
         <v>5</v>
       </c>
       <c r="F14">
-        <v>8200</v>
+        <v>3000</v>
       </c>
       <c r="H14">
         <v>10</v>
@@ -1731,7 +1731,7 @@
   <dimension ref="A1:K29"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
+      <selection activeCell="A14" sqref="A14:F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2642,8 +2642,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68AD9398-98CA-4DC9-BCD5-D6EC9B94D5CB}">
   <dimension ref="A1:K29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
- added PG&E models for liquefaction (published) - added UserDefinedGM under IM to accommodate gridded GM formats (for hazard runs) - added repair rate models - minor fixes to existing models to avoid returning zero values - general updates to improve clarity - set returns for probability to be in decimals/fractions - added north arrow to plotting under geodata
</commit_message>
<xml_diff>
--- a/param_dist/below_ground.xlsx
+++ b/param_dist/below_ground.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://slategeotech-my.sharepoint.com/personal/bzheng_slategeotech_com/Documents/CEC/OpenSRA/param_dist/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="74" documentId="13_ncr:1_{A3D454CB-C675-440C-B26E-BB3C7CD09156}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3AAC5B23-7A5E-4B88-99E3-AAC6E2F95A94}"/>
+  <xr:revisionPtr revIDLastSave="205" documentId="13_ncr:1_{A3D454CB-C675-440C-B26E-BB3C7CD09156}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{31741F41-32A3-49FD-BA8C-EA9C8EF106FC}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0CF1B192-5A29-435B-821A-1A8E6C927DCF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="3" xr2:uid="{0CF1B192-5A29-435B-821A-1A8E6C927DCF}"/>
   </bookViews>
   <sheets>
     <sheet name="level1" sheetId="1" r:id="rId1"/>
@@ -128,7 +128,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="495" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="533" uniqueCount="115">
   <si>
     <t>normal</t>
   </si>
@@ -404,6 +404,75 @@
   </si>
   <si>
     <t>theta_rake</t>
+  </si>
+  <si>
+    <t>corrosivity</t>
+  </si>
+  <si>
+    <t>soil corrosivity: &lt;=750 = high impact, &gt;1500 = low impact</t>
+  </si>
+  <si>
+    <t>ohm-cm</t>
+  </si>
+  <si>
+    <t>install_year</t>
+  </si>
+  <si>
+    <t>year of installation</t>
+  </si>
+  <si>
+    <t>pge_a</t>
+  </si>
+  <si>
+    <t>PG&amp;E model coefficent a</t>
+  </si>
+  <si>
+    <t>probability (fraction)</t>
+  </si>
+  <si>
+    <t>pge_b</t>
+  </si>
+  <si>
+    <t>pge_c</t>
+  </si>
+  <si>
+    <t>PG&amp;E model coefficent b</t>
+  </si>
+  <si>
+    <t>PG&amp;E model coefficent c</t>
+  </si>
+  <si>
+    <t>PG&amp;E model maximum magnitude scaling factor</t>
+  </si>
+  <si>
+    <t>PG&amp;E model lateral-spreading coefficient</t>
+  </si>
+  <si>
+    <t>PG&amp;E model settlement coefficent</t>
+  </si>
+  <si>
+    <t>PG&amp;E model lateral-spreading sigmaln</t>
+  </si>
+  <si>
+    <t>PG&amp;E model settlement sigmaln</t>
+  </si>
+  <si>
+    <t>msf_max</t>
+  </si>
+  <si>
+    <t>dl</t>
+  </si>
+  <si>
+    <t>sigl</t>
+  </si>
+  <si>
+    <t>ds</t>
+  </si>
+  <si>
+    <t>sigs</t>
+  </si>
+  <si>
+    <t>g</t>
   </si>
 </sst>
 </file>
@@ -799,8 +868,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38878A27-4F03-488B-A8C6-4048A6415AE1}">
   <dimension ref="A1:K29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3547,10 +3616,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C05FAA73-8B95-463E-BA46-D430429688CD}">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3675,6 +3744,206 @@
         <v>88</v>
       </c>
     </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>92</v>
+      </c>
+      <c r="B7" t="b">
+        <v>1</v>
+      </c>
+      <c r="C7" t="b">
+        <v>0</v>
+      </c>
+      <c r="D7" t="s">
+        <v>93</v>
+      </c>
+      <c r="E7" t="s">
+        <v>94</v>
+      </c>
+      <c r="F7">
+        <v>1600</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>95</v>
+      </c>
+      <c r="B8" t="b">
+        <v>1</v>
+      </c>
+      <c r="C8" t="b">
+        <v>0</v>
+      </c>
+      <c r="D8" t="s">
+        <v>96</v>
+      </c>
+      <c r="E8" t="s">
+        <v>6</v>
+      </c>
+      <c r="F8">
+        <v>1980</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>97</v>
+      </c>
+      <c r="B9" t="b">
+        <v>1</v>
+      </c>
+      <c r="C9" t="b">
+        <v>0</v>
+      </c>
+      <c r="D9" t="s">
+        <v>98</v>
+      </c>
+      <c r="E9" t="s">
+        <v>99</v>
+      </c>
+      <c r="F9" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>100</v>
+      </c>
+      <c r="B10" t="b">
+        <v>1</v>
+      </c>
+      <c r="C10" t="b">
+        <v>0</v>
+      </c>
+      <c r="D10" t="s">
+        <v>102</v>
+      </c>
+      <c r="E10" t="s">
+        <v>114</v>
+      </c>
+      <c r="F10" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>101</v>
+      </c>
+      <c r="B11" t="b">
+        <v>1</v>
+      </c>
+      <c r="C11" t="b">
+        <v>0</v>
+      </c>
+      <c r="D11" t="s">
+        <v>103</v>
+      </c>
+      <c r="E11" t="s">
+        <v>6</v>
+      </c>
+      <c r="F11" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>109</v>
+      </c>
+      <c r="B12" t="b">
+        <v>1</v>
+      </c>
+      <c r="C12" t="b">
+        <v>0</v>
+      </c>
+      <c r="D12" t="s">
+        <v>104</v>
+      </c>
+      <c r="E12" t="s">
+        <v>6</v>
+      </c>
+      <c r="F12" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>110</v>
+      </c>
+      <c r="B13" t="b">
+        <v>1</v>
+      </c>
+      <c r="C13" t="b">
+        <v>0</v>
+      </c>
+      <c r="D13" t="s">
+        <v>105</v>
+      </c>
+      <c r="E13" t="s">
+        <v>3</v>
+      </c>
+      <c r="F13" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>111</v>
+      </c>
+      <c r="B14" t="b">
+        <v>1</v>
+      </c>
+      <c r="C14" t="b">
+        <v>0</v>
+      </c>
+      <c r="D14" t="s">
+        <v>107</v>
+      </c>
+      <c r="E14" t="s">
+        <v>6</v>
+      </c>
+      <c r="F14" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>112</v>
+      </c>
+      <c r="B15" t="b">
+        <v>1</v>
+      </c>
+      <c r="C15" t="b">
+        <v>0</v>
+      </c>
+      <c r="D15" t="s">
+        <v>106</v>
+      </c>
+      <c r="E15" t="s">
+        <v>3</v>
+      </c>
+      <c r="F15" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>113</v>
+      </c>
+      <c r="B16" t="b">
+        <v>1</v>
+      </c>
+      <c r="C16" t="b">
+        <v>0</v>
+      </c>
+      <c r="D16" t="s">
+        <v>108</v>
+      </c>
+      <c r="E16" t="s">
+        <v>6</v>
+      </c>
+      <c r="F16" t="s">
+        <v>68</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>